<commit_message>
update rpharma_specs.xlsx with the latest version
</commit_message>
<xml_diff>
--- a/metadata/rpharma_specs.xlsx
+++ b/metadata/rpharma_specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bs832471\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B98A449-98E4-4220-B30A-9F1FB27BB831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5EE1790-9426-40C4-B235-0BCCADC91B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="5" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="575">
   <si>
     <t>Attribute</t>
   </si>
@@ -1633,7 +1633,9 @@
     <t>Algorithm for ADVS.AVALCAT1</t>
   </si>
   <si>
-    <t>Set to null</t>
+    <t>For Parameter Code [ADVS.PARAMCD] = 'HEIGHT':
+Set to '&gt;140 cm' when Analysis Value [ADVS.AVAL] &gt; 140,
+else set to '&lt;= 140 cm' when Analysis Value [ADVS.AVAL] &lt;= 140.</t>
   </si>
   <si>
     <t>Algorithm for ADVS.BASE</t>
@@ -1645,7 +1647,10 @@
     <t>Algorithm for ADVS.BASETYPE</t>
   </si>
   <si>
-    <t>Set to 'LAST'</t>
+    <t>Set to 'LAST: AFTER LYING DOWN FOR 5 MINUTES' when Analysis Timepoint (N) [ADVS.ATPTN]= 815,
+ else set to 'LAST: AFTER STANDING FOR 1 MINUTE' when Analysis Timepoint (N) [ADVS.ATPTN]= 816,
+ else set to 'LAST: AFTER STANDING FOR 3 MINUTES' when Analysis Timepoint (N) [ADVS.ATPTN]= 817,
+ else set to 'LAST when Analysis Timepoint (N) [ADVS.ATPTN] is missing</t>
   </si>
   <si>
     <t>Algorithm for ADVS.ABLFL</t>
@@ -1673,6 +1678,11 @@
   </si>
   <si>
     <t>Algorithm for ADVS.DTYPE</t>
+  </si>
+  <si>
+    <t>For additional summary records, set to 'AVERAGE'.
+For additional End of Treatment records, set to 'LOV'.
+Else set to null.</t>
   </si>
   <si>
     <t>Algorithm for ADVS.ANRHI</t>
@@ -1889,7 +1899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1902,7 +1912,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1918,6 +1927,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2322,21 +2337,21 @@
         <v>393</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B2" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -2451,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129AE431-5806-471D-9C82-A144A32316F7}">
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="O97" sqref="O97:O122"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="Q93" sqref="Q93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2462,7 +2477,7 @@
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="12"/>
+    <col min="6" max="6" width="9" style="11"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -2478,7 +2493,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2493,7 +2508,7 @@
       <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -2552,7 +2567,7 @@
       <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I2" t="s">
@@ -2583,7 +2598,7 @@
       <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>53</v>
       </c>
       <c r="I3" t="s">
@@ -2617,7 +2632,7 @@
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I4" t="s">
@@ -2651,7 +2666,7 @@
       <c r="E5" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>61</v>
       </c>
       <c r="I5" t="s">
@@ -2682,7 +2697,7 @@
       <c r="E6" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>5</v>
       </c>
       <c r="L6" s="3"/>
@@ -2704,7 +2719,7 @@
       <c r="E7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>10</v>
       </c>
       <c r="L7" s="3"/>
@@ -2726,7 +2741,7 @@
       <c r="E8" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>8</v>
       </c>
       <c r="L8" s="3"/>
@@ -2748,7 +2763,7 @@
       <c r="E9" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>8</v>
       </c>
       <c r="I9" t="s">
@@ -2779,7 +2794,7 @@
       <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="I10" t="s">
@@ -2813,7 +2828,7 @@
       <c r="E11" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I11" t="s">
@@ -2847,7 +2862,7 @@
       <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>61</v>
       </c>
       <c r="I12" t="s">
@@ -2884,7 +2899,7 @@
       <c r="E13" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>3</v>
       </c>
       <c r="L13" s="3"/>
@@ -2906,7 +2921,7 @@
       <c r="E14" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>8</v>
       </c>
       <c r="L14" s="3"/>
@@ -2928,7 +2943,7 @@
       <c r="E15" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I15" t="s">
@@ -2965,7 +2980,7 @@
       <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>97</v>
       </c>
       <c r="I16" t="s">
@@ -3002,7 +3017,7 @@
       <c r="E17" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I17" t="s">
@@ -3033,7 +3048,7 @@
       <c r="E18" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>105</v>
       </c>
       <c r="I18" t="s">
@@ -3067,7 +3082,7 @@
       <c r="E19" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I19" t="s">
@@ -3098,7 +3113,7 @@
       <c r="E20" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>105</v>
       </c>
       <c r="L20" s="3"/>
@@ -3120,7 +3135,7 @@
       <c r="E21" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>79</v>
       </c>
       <c r="L21" s="3"/>
@@ -3142,7 +3157,7 @@
       <c r="E22" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>117</v>
       </c>
       <c r="I22" t="s">
@@ -3213,7 +3228,7 @@
       <c r="E24" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>127</v>
       </c>
       <c r="I24" t="s">
@@ -3247,7 +3262,7 @@
       <c r="E25" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>127</v>
       </c>
       <c r="I25" t="s">
@@ -3284,7 +3299,7 @@
       <c r="E26" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I26" t="s">
@@ -3318,7 +3333,7 @@
       <c r="E27" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H27" t="s">
@@ -3355,7 +3370,7 @@
       <c r="E28" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>140</v>
       </c>
       <c r="I28" t="s">
@@ -3389,7 +3404,7 @@
       <c r="E29" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="11" t="s">
         <v>144</v>
       </c>
       <c r="I29" t="s">
@@ -3423,7 +3438,7 @@
       <c r="E30" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>140</v>
       </c>
       <c r="I30" t="s">
@@ -3457,7 +3472,7 @@
       <c r="E31" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>144</v>
       </c>
       <c r="I31" t="s">
@@ -3491,7 +3506,7 @@
       <c r="E32" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="11" t="s">
         <v>140</v>
       </c>
       <c r="I32" t="s">
@@ -3528,7 +3543,7 @@
       <c r="E33" t="s">
         <v>69</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I33" t="s">
@@ -3562,7 +3577,7 @@
       <c r="E34" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>140</v>
       </c>
       <c r="I34" t="s">
@@ -3596,7 +3611,7 @@
       <c r="E35" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I35" t="s">
@@ -3627,7 +3642,7 @@
       <c r="E36" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="11">
         <v>8</v>
       </c>
       <c r="H36" t="s">
@@ -3729,7 +3744,7 @@
       <c r="E39" t="s">
         <v>69</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H39" t="s">
@@ -3763,7 +3778,7 @@
       <c r="E40" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H40" t="s">
@@ -3797,7 +3812,7 @@
       <c r="E41" t="s">
         <v>69</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41" s="11">
         <v>8</v>
       </c>
       <c r="L41" s="3"/>
@@ -3819,7 +3834,7 @@
       <c r="E42" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="11" t="s">
         <v>127</v>
       </c>
       <c r="I42" t="s">
@@ -3853,7 +3868,7 @@
       <c r="E43" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H43" t="s">
@@ -3887,7 +3902,7 @@
       <c r="E44" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="11" t="s">
         <v>127</v>
       </c>
       <c r="I44" t="s">
@@ -3949,7 +3964,7 @@
       <c r="E46" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H46" t="s">
@@ -3983,7 +3998,7 @@
       <c r="E47" t="s">
         <v>48</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="11" t="s">
         <v>127</v>
       </c>
       <c r="I47" t="s">
@@ -4014,7 +4029,7 @@
       <c r="E48" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I48" t="s">
@@ -4045,7 +4060,7 @@
       <c r="E49" t="s">
         <v>210</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="11" t="s">
         <v>79</v>
       </c>
       <c r="G49" t="s">
@@ -4079,7 +4094,7 @@
       <c r="E50" t="s">
         <v>210</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="11" t="s">
         <v>79</v>
       </c>
       <c r="G50" t="s">
@@ -4113,7 +4128,7 @@
       <c r="E51" t="s">
         <v>69</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H51" t="s">
@@ -4137,7 +4152,7 @@
       <c r="E52" t="s">
         <v>48</v>
       </c>
-      <c r="F52" s="12">
+      <c r="F52" s="11">
         <v>40</v>
       </c>
     </row>
@@ -4158,7 +4173,7 @@
       <c r="E53" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H53" t="s">
@@ -4182,8 +4197,8 @@
       <c r="E54" t="s">
         <v>48</v>
       </c>
-      <c r="F54" s="13" t="s">
-        <v>79</v>
+      <c r="F54" s="11">
+        <v>12</v>
       </c>
       <c r="I54" t="s">
         <v>24</v>
@@ -4212,7 +4227,7 @@
       <c r="E55" t="s">
         <v>48</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F55" s="12" t="s">
         <v>222</v>
       </c>
       <c r="I55" t="s">
@@ -4242,7 +4257,7 @@
       <c r="E56" t="s">
         <v>48</v>
       </c>
-      <c r="F56" s="13" t="s">
+      <c r="F56" s="12" t="s">
         <v>222</v>
       </c>
       <c r="I56" t="s">
@@ -4272,7 +4287,7 @@
       <c r="E57" t="s">
         <v>48</v>
       </c>
-      <c r="F57" s="12">
+      <c r="F57" s="11">
         <v>20</v>
       </c>
       <c r="I57" t="s">
@@ -4302,7 +4317,7 @@
       <c r="E58" t="s">
         <v>69</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="F58" s="12" t="s">
         <v>79</v>
       </c>
       <c r="I58" t="s">
@@ -4333,7 +4348,7 @@
       <c r="E59" t="s">
         <v>48</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F59" s="12" t="s">
         <v>230</v>
       </c>
       <c r="I59" t="s">
@@ -4363,7 +4378,7 @@
       <c r="E60" t="s">
         <v>48</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F60" s="12" t="s">
         <v>232</v>
       </c>
       <c r="I60" t="s">
@@ -4393,7 +4408,7 @@
       <c r="E61" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F61" s="12" t="s">
         <v>230</v>
       </c>
       <c r="I61" t="s">
@@ -4423,7 +4438,7 @@
       <c r="E62" t="s">
         <v>69</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F62" s="12" t="s">
         <v>79</v>
       </c>
       <c r="I62" t="s">
@@ -4453,7 +4468,7 @@
       <c r="E63" t="s">
         <v>48</v>
       </c>
-      <c r="F63" s="13" t="s">
+      <c r="F63" s="12" t="s">
         <v>49</v>
       </c>
       <c r="I63" t="s">
@@ -4483,7 +4498,7 @@
       <c r="E64" t="s">
         <v>48</v>
       </c>
-      <c r="F64" s="13" t="s">
+      <c r="F64" s="12" t="s">
         <v>49</v>
       </c>
       <c r="I64" t="s">
@@ -4517,7 +4532,7 @@
       <c r="E65" t="s">
         <v>48</v>
       </c>
-      <c r="F65" s="13" t="s">
+      <c r="F65" s="12" t="s">
         <v>97</v>
       </c>
       <c r="I65" t="s">
@@ -4585,7 +4600,7 @@
       <c r="E67" t="s">
         <v>48</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="F67" s="12" t="s">
         <v>140</v>
       </c>
       <c r="I67" t="s">
@@ -4619,7 +4634,7 @@
       <c r="E68" t="s">
         <v>48</v>
       </c>
-      <c r="F68" s="13" t="s">
+      <c r="F68" s="12" t="s">
         <v>140</v>
       </c>
       <c r="I68" t="s">
@@ -4653,7 +4668,7 @@
       <c r="E69" t="s">
         <v>69</v>
       </c>
-      <c r="F69" s="13" t="s">
+      <c r="F69" s="12" t="s">
         <v>79</v>
       </c>
       <c r="H69" t="s">
@@ -4687,8 +4702,8 @@
       <c r="E70" t="s">
         <v>69</v>
       </c>
-      <c r="F70" s="13" t="s">
-        <v>79</v>
+      <c r="F70" s="4">
+        <v>8</v>
       </c>
       <c r="H70" t="s">
         <v>175</v>
@@ -4721,7 +4736,7 @@
       <c r="E71" t="s">
         <v>69</v>
       </c>
-      <c r="F71" s="13" t="s">
+      <c r="F71" s="12" t="s">
         <v>79</v>
       </c>
       <c r="H71" t="s">
@@ -4755,7 +4770,7 @@
       <c r="E72" t="s">
         <v>48</v>
       </c>
-      <c r="F72" s="12">
+      <c r="F72" s="11">
         <v>2</v>
       </c>
       <c r="I72" t="s">
@@ -4786,7 +4801,7 @@
       <c r="E73" t="s">
         <v>48</v>
       </c>
-      <c r="F73" s="12">
+      <c r="F73" s="11">
         <v>8</v>
       </c>
       <c r="I73" t="s">
@@ -4817,7 +4832,7 @@
       <c r="E74" t="s">
         <v>48</v>
       </c>
-      <c r="F74" s="12">
+      <c r="F74" s="11">
         <v>40</v>
       </c>
       <c r="I74" t="s">
@@ -4848,7 +4863,7 @@
       <c r="E75" t="s">
         <v>48</v>
       </c>
-      <c r="F75" s="12">
+      <c r="F75" s="11">
         <v>100</v>
       </c>
       <c r="I75" t="s">
@@ -4879,7 +4894,7 @@
       <c r="E76" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="12">
+      <c r="F76" s="11">
         <v>200</v>
       </c>
       <c r="I76" t="s">
@@ -4910,7 +4925,7 @@
       <c r="E77" t="s">
         <v>48</v>
       </c>
-      <c r="F77" s="12">
+      <c r="F77" s="11">
         <v>40</v>
       </c>
       <c r="I77" t="s">
@@ -4941,7 +4956,7 @@
       <c r="E78" t="s">
         <v>48</v>
       </c>
-      <c r="F78" s="12">
+      <c r="F78" s="11">
         <v>200</v>
       </c>
       <c r="I78" t="s">
@@ -4972,7 +4987,7 @@
       <c r="E79" t="s">
         <v>210</v>
       </c>
-      <c r="F79" s="12">
+      <c r="F79" s="11">
         <v>8</v>
       </c>
       <c r="I79" t="s">
@@ -5003,7 +5018,7 @@
       <c r="E80" t="s">
         <v>48</v>
       </c>
-      <c r="F80" s="12">
+      <c r="F80" s="11">
         <v>40</v>
       </c>
       <c r="I80" t="s">
@@ -5034,7 +5049,7 @@
       <c r="E81" t="s">
         <v>48</v>
       </c>
-      <c r="F81" s="12">
+      <c r="F81" s="11">
         <v>8</v>
       </c>
       <c r="I81" t="s">
@@ -5065,7 +5080,7 @@
       <c r="E82" t="s">
         <v>48</v>
       </c>
-      <c r="F82" s="12">
+      <c r="F82" s="11">
         <v>200</v>
       </c>
       <c r="I82" t="s">
@@ -5096,7 +5111,7 @@
       <c r="E83" t="s">
         <v>48</v>
       </c>
-      <c r="F83" s="14" t="s">
+      <c r="F83" s="13" t="s">
         <v>127</v>
       </c>
       <c r="G83" s="5"/>
@@ -5133,7 +5148,7 @@
       <c r="E84" t="s">
         <v>69</v>
       </c>
-      <c r="F84" s="12">
+      <c r="F84" s="11">
         <v>8</v>
       </c>
       <c r="I84" t="s">
@@ -5164,7 +5179,7 @@
       <c r="E85" t="s">
         <v>48</v>
       </c>
-      <c r="F85" s="12">
+      <c r="F85" s="11">
         <v>200</v>
       </c>
       <c r="I85" t="s">
@@ -5195,7 +5210,7 @@
       <c r="E86" t="s">
         <v>283</v>
       </c>
-      <c r="F86" s="12">
+      <c r="F86" s="11">
         <v>25</v>
       </c>
       <c r="I86" t="s">
@@ -5226,7 +5241,7 @@
       <c r="E87" t="s">
         <v>69</v>
       </c>
-      <c r="F87" s="12">
+      <c r="F87" s="11">
         <v>8</v>
       </c>
       <c r="I87" t="s">
@@ -5257,7 +5272,7 @@
       <c r="E88" t="s">
         <v>48</v>
       </c>
-      <c r="F88" s="12">
+      <c r="F88" s="11">
         <v>40</v>
       </c>
       <c r="I88" t="s">
@@ -5288,7 +5303,7 @@
       <c r="E89" t="s">
         <v>69</v>
       </c>
-      <c r="F89" s="12">
+      <c r="F89" s="11">
         <v>8</v>
       </c>
       <c r="I89" t="s">
@@ -5319,7 +5334,7 @@
       <c r="E90" t="s">
         <v>48</v>
       </c>
-      <c r="F90" s="12">
+      <c r="F90" s="11">
         <v>40</v>
       </c>
       <c r="I90" t="s">
@@ -5350,7 +5365,7 @@
       <c r="E91" t="s">
         <v>69</v>
       </c>
-      <c r="F91" s="13" t="s">
+      <c r="F91" s="12" t="s">
         <v>79</v>
       </c>
       <c r="I91" t="s">
@@ -5381,7 +5396,7 @@
       <c r="E92" t="s">
         <v>69</v>
       </c>
-      <c r="F92" s="12">
+      <c r="F92" s="11">
         <v>8</v>
       </c>
       <c r="I92" t="s">
@@ -5412,7 +5427,7 @@
       <c r="E93" t="s">
         <v>48</v>
       </c>
-      <c r="F93" s="12">
+      <c r="F93" s="11">
         <v>8</v>
       </c>
       <c r="I93" t="s">
@@ -5443,7 +5458,7 @@
       <c r="E94" t="s">
         <v>48</v>
       </c>
-      <c r="F94" s="12">
+      <c r="F94" s="11">
         <v>200</v>
       </c>
       <c r="I94" t="s">
@@ -5474,7 +5489,7 @@
       <c r="E95" t="s">
         <v>69</v>
       </c>
-      <c r="F95" s="12">
+      <c r="F95" s="11">
         <v>8</v>
       </c>
       <c r="I95" t="s">
@@ -5505,7 +5520,7 @@
       <c r="E96" t="s">
         <v>48</v>
       </c>
-      <c r="F96" s="12">
+      <c r="F96" s="11">
         <v>8</v>
       </c>
       <c r="I96" t="s">
@@ -5536,7 +5551,7 @@
       <c r="E97" t="s">
         <v>210</v>
       </c>
-      <c r="F97" s="12">
+      <c r="F97" s="11">
         <v>8</v>
       </c>
       <c r="L97" s="3"/>
@@ -5564,7 +5579,7 @@
       <c r="E98" t="s">
         <v>48</v>
       </c>
-      <c r="F98" s="12">
+      <c r="F98" s="11">
         <v>40</v>
       </c>
       <c r="L98" s="3"/>
@@ -5592,7 +5607,7 @@
       <c r="E99" t="s">
         <v>48</v>
       </c>
-      <c r="F99" s="12">
+      <c r="F99" s="11">
         <v>40</v>
       </c>
       <c r="L99" s="3"/>
@@ -5620,7 +5635,7 @@
       <c r="E100" t="s">
         <v>69</v>
       </c>
-      <c r="F100" s="12">
+      <c r="F100" s="11">
         <v>8</v>
       </c>
       <c r="L100" s="3"/>
@@ -5645,7 +5660,7 @@
       <c r="E101" t="s">
         <v>210</v>
       </c>
-      <c r="F101" s="12">
+      <c r="F101" s="11">
         <v>8</v>
       </c>
       <c r="L101" s="3"/>
@@ -5673,8 +5688,8 @@
       <c r="E102" t="s">
         <v>48</v>
       </c>
-      <c r="F102" s="12">
-        <v>30</v>
+      <c r="F102" s="11">
+        <v>36</v>
       </c>
       <c r="L102" s="3"/>
       <c r="M102" t="s">
@@ -5701,7 +5716,7 @@
       <c r="E103" t="s">
         <v>48</v>
       </c>
-      <c r="F103" s="12">
+      <c r="F103" s="11">
         <v>1</v>
       </c>
       <c r="K103" t="s">
@@ -5732,7 +5747,7 @@
       <c r="E104" t="s">
         <v>210</v>
       </c>
-      <c r="F104" s="12">
+      <c r="F104" s="11">
         <v>8</v>
       </c>
       <c r="L104" s="3"/>
@@ -5760,7 +5775,7 @@
       <c r="E105" t="s">
         <v>210</v>
       </c>
-      <c r="F105" s="12">
+      <c r="F105" s="11">
         <v>8</v>
       </c>
       <c r="L105" s="3"/>
@@ -5788,7 +5803,7 @@
       <c r="E106" t="s">
         <v>48</v>
       </c>
-      <c r="F106" s="12">
+      <c r="F106" s="11">
         <v>20</v>
       </c>
       <c r="L106" s="3"/>
@@ -5816,7 +5831,7 @@
       <c r="E107" t="s">
         <v>210</v>
       </c>
-      <c r="F107" s="12">
+      <c r="F107" s="11">
         <v>8</v>
       </c>
       <c r="L107" s="3"/>
@@ -5844,7 +5859,7 @@
       <c r="E108" t="s">
         <v>210</v>
       </c>
-      <c r="F108" s="12">
+      <c r="F108" s="11">
         <v>8</v>
       </c>
       <c r="L108" s="3"/>
@@ -5872,7 +5887,7 @@
       <c r="E109" t="s">
         <v>48</v>
       </c>
-      <c r="F109" s="12">
+      <c r="F109" s="11">
         <v>20</v>
       </c>
       <c r="L109" s="3"/>
@@ -5900,7 +5915,7 @@
       <c r="E110" t="s">
         <v>48</v>
       </c>
-      <c r="F110" s="12">
+      <c r="F110" s="11">
         <v>20</v>
       </c>
       <c r="L110" s="3"/>
@@ -5928,7 +5943,7 @@
       <c r="E111" t="s">
         <v>210</v>
       </c>
-      <c r="F111" s="12">
+      <c r="F111" s="11">
         <v>8</v>
       </c>
       <c r="L111" s="3"/>
@@ -5956,7 +5971,7 @@
       <c r="E112" t="s">
         <v>210</v>
       </c>
-      <c r="F112" s="12">
+      <c r="F112" s="11">
         <v>8</v>
       </c>
       <c r="L112" s="3"/>
@@ -5984,7 +5999,7 @@
       <c r="E113" t="s">
         <v>69</v>
       </c>
-      <c r="F113" s="12">
+      <c r="F113" s="11">
         <v>8</v>
       </c>
       <c r="L113" s="3"/>
@@ -6012,7 +6027,7 @@
       <c r="E114" t="s">
         <v>69</v>
       </c>
-      <c r="F114" s="12">
+      <c r="F114" s="11">
         <v>8</v>
       </c>
       <c r="L114" s="3"/>
@@ -6040,7 +6055,7 @@
       <c r="E115" t="s">
         <v>48</v>
       </c>
-      <c r="F115" s="12">
+      <c r="F115" s="11">
         <v>40</v>
       </c>
       <c r="L115" s="3"/>
@@ -6068,7 +6083,7 @@
       <c r="E116" t="s">
         <v>69</v>
       </c>
-      <c r="F116" s="12">
+      <c r="F116" s="11">
         <v>8</v>
       </c>
       <c r="L116" s="3"/>
@@ -6096,7 +6111,7 @@
       <c r="E117" t="s">
         <v>48</v>
       </c>
-      <c r="F117" s="12">
+      <c r="F117" s="11">
         <v>200</v>
       </c>
       <c r="L117" s="3"/>
@@ -6124,7 +6139,7 @@
       <c r="E118" t="s">
         <v>69</v>
       </c>
-      <c r="F118" s="12">
+      <c r="F118" s="11">
         <v>8</v>
       </c>
       <c r="L118" s="3"/>
@@ -6152,7 +6167,7 @@
       <c r="E119" t="s">
         <v>48</v>
       </c>
-      <c r="F119" s="12">
+      <c r="F119" s="11">
         <v>200</v>
       </c>
       <c r="L119" s="3"/>
@@ -6180,7 +6195,7 @@
       <c r="E120" t="s">
         <v>48</v>
       </c>
-      <c r="F120" s="12">
+      <c r="F120" s="11">
         <v>200</v>
       </c>
       <c r="L120" s="3"/>
@@ -6208,7 +6223,7 @@
       <c r="E121" t="s">
         <v>48</v>
       </c>
-      <c r="F121" s="12">
+      <c r="F121" s="11">
         <v>1</v>
       </c>
       <c r="K121" t="s">
@@ -6239,7 +6254,7 @@
       <c r="E122" t="s">
         <v>48</v>
       </c>
-      <c r="F122" s="12">
+      <c r="F122" s="11">
         <v>1</v>
       </c>
       <c r="K122" t="s">
@@ -8109,18 +8124,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A27F77-A36A-4B0F-AB98-73EE4727DE22}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="148.5703125" customWidth="1"/>
+    <col min="4" max="4" width="148.5703125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8133,7 +8148,7 @@
       <c r="C1" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>501</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -8159,7 +8174,7 @@
       <c r="C2" t="s">
         <v>507</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>508</v>
       </c>
     </row>
@@ -8173,7 +8188,7 @@
       <c r="C3" t="s">
         <v>507</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>511</v>
       </c>
     </row>
@@ -8317,7 +8332,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="45.75">
       <c r="A14" t="s">
         <v>323</v>
       </c>
@@ -8331,7 +8346,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="24">
       <c r="A15" t="s">
         <v>328</v>
       </c>
@@ -8345,7 +8360,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="58.5" customHeight="1">
       <c r="A16" t="s">
         <v>331</v>
       </c>
@@ -8359,7 +8374,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="42.75">
+    <row r="17" spans="1:4" ht="45.75">
       <c r="A17" t="s">
         <v>334</v>
       </c>
@@ -8373,7 +8388,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="39.4">
+    <row r="18" spans="1:4" ht="36">
       <c r="A18" t="s">
         <v>337</v>
       </c>
@@ -8383,11 +8398,11 @@
       <c r="C18" t="s">
         <v>507</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="91.15">
+    <row r="19" spans="1:4" ht="84">
       <c r="A19" t="s">
         <v>340</v>
       </c>
@@ -8397,11 +8412,11 @@
       <c r="C19" t="s">
         <v>507</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="45.75">
       <c r="A20" t="s">
         <v>343</v>
       </c>
@@ -8411,90 +8426,92 @@
       <c r="C20" t="s">
         <v>507</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" ht="57.2">
+      <c r="D20" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60.75">
       <c r="A21" t="s">
         <v>346</v>
       </c>
       <c r="B21" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C21" t="s">
         <v>507</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="57.2">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60.75">
       <c r="A22" t="s">
         <v>349</v>
       </c>
       <c r="B22" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C22" t="s">
         <v>507</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="128.44999999999999">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="137.25">
       <c r="A23" t="s">
         <v>352</v>
       </c>
       <c r="B23" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C23" t="s">
         <v>507</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30.75">
       <c r="A24" t="s">
         <v>355</v>
       </c>
       <c r="B24" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C24" t="s">
         <v>507</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="57.2">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="60.75">
       <c r="A25" t="s">
         <v>358</v>
       </c>
       <c r="B25" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C25" t="s">
         <v>507</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="57.2">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60.75">
       <c r="A26" t="s">
         <v>361</v>
       </c>
       <c r="B26" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C26" t="s">
         <v>507</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -8502,27 +8519,27 @@
         <v>364</v>
       </c>
       <c r="B27" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C27" t="s">
         <v>507</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="42.75">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="45.75">
       <c r="A28" t="s">
         <v>367</v>
       </c>
       <c r="B28" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C28" t="s">
         <v>507</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -8530,13 +8547,13 @@
         <v>370</v>
       </c>
       <c r="B29" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C29" t="s">
         <v>507</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -8544,13 +8561,13 @@
         <v>373</v>
       </c>
       <c r="B30" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C30" t="s">
         <v>507</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -8558,27 +8575,27 @@
         <v>376</v>
       </c>
       <c r="B31" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C31" t="s">
         <v>507</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.5">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30.75">
       <c r="A32" t="s">
         <v>379</v>
       </c>
       <c r="B32" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C32" t="s">
         <v>507</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -8586,13 +8603,13 @@
         <v>382</v>
       </c>
       <c r="B33" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C33" t="s">
         <v>507</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -8600,100 +8617,43 @@
         <v>385</v>
       </c>
       <c r="B34" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C34" t="s">
         <v>507</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="85.7">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="91.5">
       <c r="A35" t="s">
         <v>388</v>
       </c>
       <c r="B35" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C35" t="s">
         <v>507</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.5">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30.75">
       <c r="A36" t="s">
         <v>391</v>
       </c>
       <c r="B36" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C36" t="s">
         <v>507</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15"/>
-    <row r="38" spans="1:4" ht="15"/>
-    <row r="39" spans="1:4" ht="15"/>
-    <row r="40" spans="1:4" ht="15"/>
-    <row r="41" spans="1:4" ht="15"/>
-    <row r="42" spans="1:4" ht="15"/>
-    <row r="43" spans="1:4" ht="15"/>
-    <row r="44" spans="1:4" ht="15"/>
-    <row r="45" spans="1:4" ht="15"/>
-    <row r="46" spans="1:4" ht="15"/>
-    <row r="47" spans="1:4" ht="15"/>
-    <row r="48" spans="1:4" ht="15"/>
-    <row r="49" ht="15"/>
-    <row r="50" ht="15"/>
-    <row r="51" ht="15"/>
-    <row r="52" ht="15"/>
-    <row r="53" ht="15"/>
-    <row r="54" ht="15"/>
-    <row r="55" ht="15"/>
-    <row r="56" ht="15"/>
-    <row r="57" ht="15"/>
-    <row r="58" ht="15"/>
-    <row r="60" ht="15"/>
-    <row r="61" ht="15"/>
-    <row r="62" ht="15"/>
-    <row r="63" ht="15"/>
-    <row r="64" ht="15"/>
-    <row r="65" ht="15"/>
-    <row r="66" ht="15"/>
-    <row r="67" ht="15"/>
-    <row r="68" ht="15"/>
-    <row r="69" ht="15"/>
-    <row r="70" ht="15"/>
-    <row r="71" ht="15"/>
-    <row r="72" ht="15"/>
-    <row r="73" ht="15"/>
-    <row r="74" ht="15"/>
-    <row r="75" ht="15"/>
-    <row r="76" ht="15"/>
-    <row r="77" ht="15"/>
-    <row r="78" ht="15"/>
-    <row r="79" ht="15"/>
-    <row r="80" ht="15"/>
-    <row r="81" ht="15"/>
-    <row r="82" ht="15"/>
-    <row r="83" ht="15"/>
-    <row r="84" ht="15"/>
-    <row r="85" ht="15"/>
-    <row r="86" ht="15"/>
-    <row r="87" ht="15"/>
-    <row r="88" ht="15"/>
-    <row r="89" ht="15"/>
-    <row r="90" ht="15"/>
-    <row r="91" ht="15"/>
-    <row r="92" ht="15"/>
-    <row r="93" ht="15"/>
-    <row r="94" ht="15"/>
+        <v>569</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: cleaning up sections and numbering; feat: Flagging variables for pops and time imputation
</commit_message>
<xml_diff>
--- a/metadata/rpharma_specs.xlsx
+++ b/metadata/rpharma_specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phuseaccount.sharepoint.com/sites/Pharmaverse-admiral/Shared Documents/RPharma2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="400" documentId="13_ncr:1_{7D220467-D1C0-4B22-9952-64DAEB9CC36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E528757B-A6F2-4DB7-91F4-C5DD949A064E}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="13_ncr:1_{7D220467-D1C0-4B22-9952-64DAEB9CC36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB3B545-E298-425B-9013-DB72E7452093}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Documents!$A$1:$C$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Study!$A$1:$B$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$R$102</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$S$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$S$121</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="585">
   <si>
     <t>Attribute</t>
   </si>
@@ -1822,6 +1822,33 @@
   </si>
   <si>
     <t>AGEGR1</t>
+  </si>
+  <si>
+    <t>TRTSTMF</t>
+  </si>
+  <si>
+    <t>TRTETMF</t>
+  </si>
+  <si>
+    <t>Time 1st Exposure Period Imput. Flag</t>
+  </si>
+  <si>
+    <t>Time Last Exposure Period Imput. Flag</t>
+  </si>
+  <si>
+    <t>Imputation</t>
+  </si>
+  <si>
+    <t>TRTSTMF= H if the entire time is imputed. TRTSTMF = M if minutes and seconds are imputed. TRTSTMF = S if only seconds are imputed.</t>
+  </si>
+  <si>
+    <t>TRTETMF= H if the entire time is imputed. TRTETMF = M if minutes and seconds are imputed. TRTETMF = S if only seconds are imputed.</t>
+  </si>
+  <si>
+    <t>ADSL.TRTSTMF</t>
+  </si>
+  <si>
+    <t>ADSL.TRTETMF</t>
   </si>
 </sst>
 </file>
@@ -2478,10 +2505,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129AE431-5806-471D-9C82-A144A32316F7}">
-  <dimension ref="A1:S119"/>
+  <dimension ref="A1:S121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2597,7 +2624,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <f t="shared" ref="A3:A63" si="0">A2+1</f>
+        <f t="shared" ref="A3:A65" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -3595,19 +3622,16 @@
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>159</v>
+        <v>576</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>578</v>
       </c>
       <c r="E34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H34" t="s">
-        <v>118</v>
+        <v>48</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
       </c>
       <c r="I34" t="s">
         <v>25</v>
@@ -3617,7 +3641,7 @@
         <v>77</v>
       </c>
       <c r="O34" t="s">
-        <v>161</v>
+        <v>583</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3629,10 +3653,10 @@
         <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E35" t="s">
         <v>69</v>
@@ -3641,7 +3665,7 @@
         <v>76</v>
       </c>
       <c r="H35" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="I35" t="s">
         <v>25</v>
@@ -3651,7 +3675,7 @@
         <v>77</v>
       </c>
       <c r="O35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3663,23 +3687,29 @@
         <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>574</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E36" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="11">
-        <v>8</v>
+      <c r="F36" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" t="s">
+        <v>25</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" t="s">
         <v>77</v>
       </c>
       <c r="O36" t="s">
-        <v>550</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -3691,19 +3721,16 @@
         <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>166</v>
+        <v>577</v>
       </c>
       <c r="D37" t="s">
-        <v>167</v>
+        <v>579</v>
       </c>
       <c r="E37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H37" t="s">
-        <v>118</v>
+        <v>48</v>
+      </c>
+      <c r="F37" s="11">
+        <v>1</v>
       </c>
       <c r="I37" t="s">
         <v>25</v>
@@ -3713,7 +3740,7 @@
         <v>77</v>
       </c>
       <c r="O37" t="s">
-        <v>168</v>
+        <v>584</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3725,29 +3752,26 @@
         <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>574</v>
       </c>
       <c r="D38" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>112</v>
+        <v>69</v>
+      </c>
+      <c r="F38" s="11">
+        <v>8</v>
       </c>
       <c r="I38" t="s">
         <v>25</v>
       </c>
-      <c r="K38" t="s">
-        <v>171</v>
-      </c>
       <c r="L38" s="3"/>
       <c r="M38" t="s">
-        <v>44</v>
-      </c>
-      <c r="P38" t="s">
-        <v>172</v>
+        <v>77</v>
+      </c>
+      <c r="O38" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3759,12 +3783,30 @@
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>563</v>
+        <v>166</v>
       </c>
       <c r="D39" t="s">
-        <v>564</v>
+        <v>167</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" t="s">
+        <v>118</v>
+      </c>
+      <c r="I39" t="s">
+        <v>25</v>
       </c>
       <c r="L39" s="3"/>
+      <c r="M39" t="s">
+        <v>77</v>
+      </c>
+      <c r="O39" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
@@ -3775,12 +3817,30 @@
         <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>565</v>
+        <v>169</v>
       </c>
       <c r="D40" t="s">
-        <v>566</v>
+        <v>170</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" t="s">
+        <v>25</v>
+      </c>
+      <c r="K40" t="s">
+        <v>171</v>
       </c>
       <c r="L40" s="3"/>
+      <c r="M40" t="s">
+        <v>44</v>
+      </c>
+      <c r="P40" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
@@ -3791,10 +3851,19 @@
         <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D41" t="s">
-        <v>569</v>
+        <v>564</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="11">
+        <v>8</v>
+      </c>
+      <c r="I41" t="s">
+        <v>25</v>
       </c>
       <c r="L41" s="3"/>
     </row>
@@ -3807,10 +3876,16 @@
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D42" t="s">
-        <v>570</v>
+        <v>566</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I42" t="s">
+        <v>25</v>
       </c>
       <c r="L42" s="3"/>
     </row>
@@ -3823,10 +3898,16 @@
         <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D43" t="s">
-        <v>572</v>
+        <v>569</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" t="s">
+        <v>25</v>
       </c>
       <c r="L43" s="3"/>
     </row>
@@ -3839,27 +3920,18 @@
         <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="D44" t="s">
-        <v>174</v>
+        <v>570</v>
       </c>
       <c r="E44" t="s">
-        <v>69</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="I44" t="s">
         <v>25</v>
       </c>
       <c r="L44" s="3"/>
-      <c r="M44" t="s">
-        <v>77</v>
-      </c>
-      <c r="O44" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
@@ -3870,30 +3942,18 @@
         <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>176</v>
+        <v>571</v>
       </c>
       <c r="D45" t="s">
-        <v>177</v>
+        <v>572</v>
       </c>
       <c r="E45" t="s">
-        <v>178</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="I45" t="s">
         <v>25</v>
       </c>
       <c r="L45" s="3"/>
-      <c r="M45" t="s">
-        <v>77</v>
-      </c>
-      <c r="O45" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
@@ -3904,19 +3964,16 @@
         <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E46" t="s">
-        <v>178</v>
+        <v>69</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="G46" t="s">
-        <v>112</v>
       </c>
       <c r="I46" t="s">
         <v>25</v>
@@ -3926,7 +3983,7 @@
         <v>77</v>
       </c>
       <c r="O46" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3938,19 +3995,29 @@
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D47" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E47" t="s">
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H47" t="s">
-        <v>157</v>
+      <c r="G47" t="s">
+        <v>112</v>
+      </c>
+      <c r="I47" t="s">
+        <v>25</v>
+      </c>
+      <c r="L47" s="3"/>
+      <c r="M47" t="s">
+        <v>77</v>
+      </c>
+      <c r="O47" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3962,19 +4029,29 @@
         <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>561</v>
+        <v>180</v>
       </c>
       <c r="D48" t="s">
-        <v>562</v>
+        <v>181</v>
       </c>
       <c r="E48" t="s">
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="F48" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H48" t="s">
-        <v>157</v>
+      <c r="G48" t="s">
+        <v>112</v>
+      </c>
+      <c r="I48" t="s">
+        <v>25</v>
+      </c>
+      <c r="L48" s="3"/>
+      <c r="M48" t="s">
+        <v>77</v>
+      </c>
+      <c r="O48" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3986,16 +4063,22 @@
         <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D49" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E49" t="s">
-        <v>48</v>
-      </c>
-      <c r="F49" s="11">
-        <v>40</v>
+        <v>69</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" t="s">
+        <v>157</v>
+      </c>
+      <c r="I49" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -4007,10 +4090,10 @@
         <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>187</v>
+        <v>561</v>
       </c>
       <c r="D50" t="s">
-        <v>188</v>
+        <v>562</v>
       </c>
       <c r="E50" t="s">
         <v>69</v>
@@ -4020,6 +4103,9 @@
       </c>
       <c r="H50" t="s">
         <v>157</v>
+      </c>
+      <c r="I50" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -4028,28 +4114,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s">
-        <v>47</v>
+        <v>186</v>
       </c>
       <c r="E51" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="11">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="I51" t="s">
-        <v>24</v>
-      </c>
-      <c r="M51" t="s">
-        <v>44</v>
-      </c>
-      <c r="P51" t="s">
-        <v>189</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -4058,28 +4138,25 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>187</v>
       </c>
       <c r="D52" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="E52" t="s">
-        <v>48</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>190</v>
+        <v>69</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H52" t="s">
+        <v>157</v>
       </c>
       <c r="I52" t="s">
-        <v>24</v>
-      </c>
-      <c r="M52" t="s">
-        <v>44</v>
-      </c>
-      <c r="P52" t="s">
-        <v>191</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -4091,25 +4168,25 @@
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E53" t="s">
         <v>48</v>
       </c>
-      <c r="F53" s="12" t="s">
-        <v>190</v>
+      <c r="F53" s="11">
+        <v>12</v>
       </c>
       <c r="I53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M53" t="s">
         <v>44</v>
       </c>
       <c r="P53" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4121,25 +4198,25 @@
         <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E54" t="s">
         <v>48</v>
       </c>
-      <c r="F54" s="11">
-        <v>20</v>
+      <c r="F54" s="12" t="s">
+        <v>190</v>
       </c>
       <c r="I54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M54" t="s">
         <v>44</v>
       </c>
       <c r="P54" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4151,26 +4228,25 @@
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>194</v>
+        <v>56</v>
       </c>
       <c r="D55" t="s">
-        <v>195</v>
+        <v>57</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>76</v>
+        <v>190</v>
       </c>
       <c r="I55" t="s">
         <v>25</v>
       </c>
-      <c r="L55" s="3"/>
       <c r="M55" t="s">
-        <v>77</v>
-      </c>
-      <c r="O55" t="s">
-        <v>196</v>
+        <v>44</v>
+      </c>
+      <c r="P55" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4182,16 +4258,16 @@
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D56" t="s">
-        <v>197</v>
+        <v>60</v>
       </c>
       <c r="E56" t="s">
         <v>48</v>
       </c>
-      <c r="F56" s="12" t="s">
-        <v>198</v>
+      <c r="F56" s="11">
+        <v>20</v>
       </c>
       <c r="I56" t="s">
         <v>25</v>
@@ -4200,7 +4276,7 @@
         <v>44</v>
       </c>
       <c r="P56" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4212,25 +4288,26 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>194</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="E57" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>200</v>
+        <v>76</v>
       </c>
       <c r="I57" t="s">
         <v>25</v>
       </c>
+      <c r="L57" s="3"/>
       <c r="M57" t="s">
-        <v>44</v>
-      </c>
-      <c r="P57" t="s">
-        <v>201</v>
+        <v>77</v>
+      </c>
+      <c r="O57" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4242,10 +4319,10 @@
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="E58" t="s">
         <v>48</v>
@@ -4260,7 +4337,7 @@
         <v>44</v>
       </c>
       <c r="P58" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4272,25 +4349,25 @@
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E59" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>76</v>
+        <v>200</v>
       </c>
       <c r="I59" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M59" t="s">
         <v>44</v>
       </c>
       <c r="P59" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -4302,25 +4379,25 @@
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="D60" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="E60" t="s">
         <v>48</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>49</v>
+        <v>198</v>
       </c>
       <c r="I60" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M60" t="s">
         <v>44</v>
       </c>
       <c r="P60" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -4332,29 +4409,25 @@
         <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E61" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="I61" t="s">
         <v>24</v>
       </c>
-      <c r="K61" t="s">
-        <v>85</v>
-      </c>
-      <c r="L61" s="3"/>
       <c r="M61" t="s">
         <v>44</v>
       </c>
       <c r="P61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -4366,29 +4439,25 @@
         <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D62" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E62" t="s">
         <v>48</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="I62" t="s">
         <v>24</v>
       </c>
-      <c r="K62" t="s">
-        <v>90</v>
-      </c>
-      <c r="L62" s="3"/>
       <c r="M62" t="s">
         <v>44</v>
       </c>
       <c r="P62" t="s">
-        <v>205</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -4397,134 +4466,134 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D63" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="E63" t="s">
         <v>48</v>
       </c>
-      <c r="F63" s="4">
-        <v>1</v>
+      <c r="F63" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="I63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K63" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="L63" s="3"/>
       <c r="M63" t="s">
         <v>44</v>
       </c>
       <c r="P63" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <f t="shared" ref="A64:A119" si="1">A63+1</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="D64" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="E64" t="s">
         <v>48</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="I64" t="s">
         <v>24</v>
       </c>
       <c r="K64" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="L64" s="3"/>
       <c r="M64" t="s">
         <v>44</v>
       </c>
       <c r="P64" t="s">
-        <v>138</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="E65" t="s">
         <v>48</v>
       </c>
-      <c r="F65" s="12" t="s">
-        <v>122</v>
+      <c r="F65" s="4">
+        <v>1</v>
       </c>
       <c r="I65" t="s">
         <v>25</v>
       </c>
       <c r="K65" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="L65" s="3"/>
       <c r="M65" t="s">
         <v>44</v>
       </c>
       <c r="P65" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A66:A121" si="1">A65+1</f>
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D66" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E66" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H66" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I66" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="K66" t="s">
+        <v>137</v>
       </c>
       <c r="L66" s="3"/>
       <c r="M66" t="s">
         <v>44</v>
       </c>
       <c r="P66" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -4536,29 +4605,29 @@
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D67" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="E67" t="s">
-        <v>69</v>
-      </c>
-      <c r="F67" s="4">
-        <v>8</v>
-      </c>
-      <c r="H67" t="s">
-        <v>157</v>
+        <v>48</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="I67" t="s">
         <v>25</v>
+      </c>
+      <c r="K67" t="s">
+        <v>137</v>
       </c>
       <c r="L67" s="3"/>
       <c r="M67" t="s">
         <v>44</v>
       </c>
       <c r="P67" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -4570,10 +4639,10 @@
         <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D68" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="E68" t="s">
         <v>69</v>
@@ -4592,7 +4661,7 @@
         <v>44</v>
       </c>
       <c r="P68" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -4604,16 +4673,19 @@
         <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="D69" t="s">
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="E69" t="s">
-        <v>48</v>
-      </c>
-      <c r="F69" s="11">
-        <v>2</v>
+        <v>69</v>
+      </c>
+      <c r="F69" s="4">
+        <v>8</v>
+      </c>
+      <c r="H69" t="s">
+        <v>157</v>
       </c>
       <c r="I69" t="s">
         <v>25</v>
@@ -4623,7 +4695,7 @@
         <v>44</v>
       </c>
       <c r="P69" t="s">
-        <v>209</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -4635,16 +4707,19 @@
         <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>159</v>
       </c>
       <c r="D70" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="E70" t="s">
-        <v>48</v>
-      </c>
-      <c r="F70" s="11">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H70" t="s">
+        <v>118</v>
       </c>
       <c r="I70" t="s">
         <v>25</v>
@@ -4654,7 +4729,7 @@
         <v>44</v>
       </c>
       <c r="P70" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -4666,16 +4741,16 @@
         <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E71" t="s">
         <v>48</v>
       </c>
       <c r="F71" s="11">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="I71" t="s">
         <v>25</v>
@@ -4685,7 +4760,7 @@
         <v>44</v>
       </c>
       <c r="P71" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -4697,16 +4772,16 @@
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D72" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E72" t="s">
         <v>48</v>
       </c>
       <c r="F72" s="11">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="I72" t="s">
         <v>25</v>
@@ -4716,7 +4791,7 @@
         <v>44</v>
       </c>
       <c r="P72" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -4728,16 +4803,16 @@
         <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E73" t="s">
         <v>48</v>
       </c>
       <c r="F73" s="11">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="I73" t="s">
         <v>25</v>
@@ -4747,7 +4822,7 @@
         <v>44</v>
       </c>
       <c r="P73" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -4759,16 +4834,16 @@
         <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E74" t="s">
         <v>48</v>
       </c>
       <c r="F74" s="11">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="I74" t="s">
         <v>25</v>
@@ -4778,7 +4853,7 @@
         <v>44</v>
       </c>
       <c r="P74" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -4790,10 +4865,10 @@
         <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E75" t="s">
         <v>48</v>
@@ -4809,7 +4884,7 @@
         <v>44</v>
       </c>
       <c r="P75" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -4821,16 +4896,16 @@
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D76" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E76" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F76" s="11">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I76" t="s">
         <v>25</v>
@@ -4840,7 +4915,7 @@
         <v>44</v>
       </c>
       <c r="P76" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -4852,16 +4927,16 @@
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E77" t="s">
         <v>48</v>
       </c>
       <c r="F77" s="11">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="I77" t="s">
         <v>25</v>
@@ -4871,7 +4946,7 @@
         <v>44</v>
       </c>
       <c r="P77" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -4883,13 +4958,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E78" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="F78" s="11">
         <v>8</v>
@@ -4902,7 +4977,7 @@
         <v>44</v>
       </c>
       <c r="P78" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -4914,16 +4989,16 @@
         <v>19</v>
       </c>
       <c r="C79" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D79" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E79" t="s">
         <v>48</v>
       </c>
       <c r="F79" s="11">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="I79" t="s">
         <v>25</v>
@@ -4933,7 +5008,7 @@
         <v>44</v>
       </c>
       <c r="P79" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -4941,36 +5016,30 @@
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" t="s">
         <v>19</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>241</v>
+      <c r="C80" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" t="s">
+        <v>235</v>
       </c>
       <c r="E80" t="s">
         <v>48</v>
       </c>
-      <c r="F80" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5" t="s">
+      <c r="F80" s="11">
+        <v>8</v>
+      </c>
+      <c r="I80" t="s">
         <v>25</v>
       </c>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="5" t="s">
+      <c r="L80" s="3"/>
+      <c r="M80" t="s">
         <v>44</v>
       </c>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-      <c r="P80" s="5" t="s">
-        <v>242</v>
+      <c r="P80" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -4978,20 +5047,20 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" t="s">
         <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D81" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E81" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F81" s="11">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="I81" t="s">
         <v>25</v>
@@ -5001,7 +5070,7 @@
         <v>44</v>
       </c>
       <c r="P81" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -5009,30 +5078,36 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C82" t="s">
-        <v>246</v>
-      </c>
-      <c r="D82" t="s">
-        <v>247</v>
+      <c r="C82" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="E82" t="s">
         <v>48</v>
       </c>
-      <c r="F82" s="11">
-        <v>200</v>
-      </c>
-      <c r="I82" t="s">
+      <c r="F82" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L82" s="3"/>
-      <c r="M82" t="s">
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P82" t="s">
-        <v>248</v>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5"/>
+      <c r="P82" s="5" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -5044,16 +5119,16 @@
         <v>19</v>
       </c>
       <c r="C83" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D83" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E83" t="s">
-        <v>251</v>
+        <v>69</v>
       </c>
       <c r="F83" s="11">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="I83" t="s">
         <v>25</v>
@@ -5063,7 +5138,7 @@
         <v>44</v>
       </c>
       <c r="P83" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -5075,16 +5150,16 @@
         <v>19</v>
       </c>
       <c r="C84" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D84" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E84" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F84" s="11">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="I84" t="s">
         <v>25</v>
@@ -5094,7 +5169,7 @@
         <v>44</v>
       </c>
       <c r="P84" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -5106,16 +5181,16 @@
         <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E85" t="s">
-        <v>48</v>
+        <v>251</v>
       </c>
       <c r="F85" s="11">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="I85" t="s">
         <v>25</v>
@@ -5125,7 +5200,7 @@
         <v>44</v>
       </c>
       <c r="P85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -5137,10 +5212,10 @@
         <v>19</v>
       </c>
       <c r="C86" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D86" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E86" t="s">
         <v>69</v>
@@ -5156,7 +5231,7 @@
         <v>44</v>
       </c>
       <c r="P86" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -5168,10 +5243,10 @@
         <v>19</v>
       </c>
       <c r="C87" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D87" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E87" t="s">
         <v>48</v>
@@ -5187,7 +5262,7 @@
         <v>44</v>
       </c>
       <c r="P87" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -5199,16 +5274,16 @@
         <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D88" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E88" t="s">
         <v>69</v>
       </c>
-      <c r="F88" s="12" t="s">
-        <v>76</v>
+      <c r="F88" s="11">
+        <v>8</v>
       </c>
       <c r="I88" t="s">
         <v>25</v>
@@ -5218,7 +5293,7 @@
         <v>44</v>
       </c>
       <c r="P88" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -5230,16 +5305,16 @@
         <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D89" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E89" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F89" s="11">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I89" t="s">
         <v>25</v>
@@ -5249,7 +5324,7 @@
         <v>44</v>
       </c>
       <c r="P89" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -5261,16 +5336,16 @@
         <v>19</v>
       </c>
       <c r="C90" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D90" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E90" t="s">
-        <v>48</v>
-      </c>
-      <c r="F90" s="11">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="I90" t="s">
         <v>25</v>
@@ -5280,7 +5355,7 @@
         <v>44</v>
       </c>
       <c r="P90" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -5292,26 +5367,26 @@
         <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D91" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E91" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F91" s="11">
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="I91" t="s">
-        <v>24</v>
-      </c>
-      <c r="K91" t="s">
-        <v>276</v>
+        <v>25</v>
       </c>
       <c r="L91" s="3"/>
       <c r="M91" t="s">
-        <v>79</v>
+        <v>44</v>
+      </c>
+      <c r="P91" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -5323,13 +5398,13 @@
         <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D92" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E92" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F92" s="11">
         <v>8</v>
@@ -5337,12 +5412,12 @@
       <c r="I92" t="s">
         <v>25</v>
       </c>
-      <c r="K92" t="s">
-        <v>279</v>
-      </c>
       <c r="L92" s="3"/>
       <c r="M92" t="s">
-        <v>79</v>
+        <v>44</v>
+      </c>
+      <c r="P92" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -5354,22 +5429,22 @@
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D93" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E93" t="s">
         <v>48</v>
       </c>
       <c r="F93" s="11">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="I93" t="s">
         <v>24</v>
       </c>
       <c r="K93" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="L93" s="3"/>
       <c r="M93" t="s">
@@ -5385,23 +5460,26 @@
         <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D94" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E94" t="s">
-        <v>178</v>
+        <v>69</v>
       </c>
       <c r="F94" s="11">
         <v>8</v>
       </c>
+      <c r="I94" t="s">
+        <v>25</v>
+      </c>
+      <c r="K94" t="s">
+        <v>279</v>
+      </c>
       <c r="L94" s="3"/>
       <c r="M94" t="s">
-        <v>77</v>
-      </c>
-      <c r="O94" t="s">
-        <v>285</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -5413,23 +5491,26 @@
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D95" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E95" t="s">
         <v>48</v>
       </c>
       <c r="F95" s="11">
-        <v>40</v>
+        <v>8</v>
+      </c>
+      <c r="I95" t="s">
+        <v>24</v>
+      </c>
+      <c r="K95" t="s">
+        <v>282</v>
       </c>
       <c r="L95" s="3"/>
       <c r="M95" t="s">
         <v>79</v>
-      </c>
-      <c r="O95" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -5441,23 +5522,23 @@
         <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D96" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E96" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="F96" s="11">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="L96" s="3"/>
       <c r="M96" t="s">
         <v>77</v>
       </c>
       <c r="O96" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -5469,20 +5550,23 @@
         <v>19</v>
       </c>
       <c r="C97" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D97" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E97" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F97" s="11">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="L97" s="3"/>
       <c r="M97" t="s">
         <v>79</v>
+      </c>
+      <c r="O97" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
@@ -5494,23 +5578,23 @@
         <v>19</v>
       </c>
       <c r="C98" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D98" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E98" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F98" s="11">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="L98" s="3"/>
       <c r="M98" t="s">
         <v>77</v>
       </c>
       <c r="O98" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -5522,23 +5606,20 @@
         <v>19</v>
       </c>
       <c r="C99" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D99" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E99" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F99" s="11">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="L99" s="3"/>
       <c r="M99" t="s">
         <v>79</v>
-      </c>
-      <c r="O99" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -5550,26 +5631,23 @@
         <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D100" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E100" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="F100" s="11">
-        <v>1</v>
-      </c>
-      <c r="K100" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="L100" s="3"/>
       <c r="M100" t="s">
         <v>77</v>
       </c>
       <c r="O100" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -5581,23 +5659,23 @@
         <v>19</v>
       </c>
       <c r="C101" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D101" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E101" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F101" s="11">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="L101" s="3"/>
       <c r="M101" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O101" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -5609,23 +5687,26 @@
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D102" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E102" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F102" s="11">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="K102" t="s">
+        <v>107</v>
       </c>
       <c r="L102" s="3"/>
       <c r="M102" t="s">
         <v>77</v>
       </c>
       <c r="O102" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -5637,23 +5718,23 @@
         <v>19</v>
       </c>
       <c r="C103" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D103" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E103" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="F103" s="11">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L103" s="3"/>
       <c r="M103" t="s">
         <v>77</v>
       </c>
       <c r="O103" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -5665,10 +5746,10 @@
         <v>19</v>
       </c>
       <c r="C104" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D104" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E104" t="s">
         <v>178</v>
@@ -5678,10 +5759,10 @@
       </c>
       <c r="L104" s="3"/>
       <c r="M104" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O104" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -5693,23 +5774,23 @@
         <v>19</v>
       </c>
       <c r="C105" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D105" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E105" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F105" s="11">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L105" s="3"/>
       <c r="M105" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O105" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -5721,23 +5802,23 @@
         <v>19</v>
       </c>
       <c r="C106" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D106" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E106" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="F106" s="11">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L106" s="3"/>
       <c r="M106" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O106" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
@@ -5749,23 +5830,23 @@
         <v>19</v>
       </c>
       <c r="C107" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D107" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E107" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="F107" s="11">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L107" s="3"/>
       <c r="M107" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O107" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -5777,23 +5858,23 @@
         <v>19</v>
       </c>
       <c r="C108" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D108" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E108" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F108" s="11">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L108" s="3"/>
       <c r="M108" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O108" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
@@ -5805,23 +5886,23 @@
         <v>19</v>
       </c>
       <c r="C109" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D109" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E109" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F109" s="11">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L109" s="3"/>
       <c r="M109" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O109" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -5833,23 +5914,23 @@
         <v>19</v>
       </c>
       <c r="C110" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D110" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E110" t="s">
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="F110" s="11">
         <v>8</v>
       </c>
       <c r="L110" s="3"/>
       <c r="M110" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O110" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -5861,23 +5942,23 @@
         <v>19</v>
       </c>
       <c r="C111" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D111" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E111" t="s">
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="F111" s="11">
         <v>8</v>
       </c>
       <c r="L111" s="3"/>
       <c r="M111" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O111" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -5889,23 +5970,23 @@
         <v>19</v>
       </c>
       <c r="C112" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D112" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E112" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F112" s="11">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="L112" s="3"/>
       <c r="M112" t="s">
         <v>77</v>
       </c>
       <c r="O112" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -5917,10 +5998,10 @@
         <v>19</v>
       </c>
       <c r="C113" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D113" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E113" t="s">
         <v>69</v>
@@ -5930,10 +6011,10 @@
       </c>
       <c r="L113" s="3"/>
       <c r="M113" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O113" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -5945,23 +6026,23 @@
         <v>19</v>
       </c>
       <c r="C114" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D114" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E114" t="s">
         <v>48</v>
       </c>
       <c r="F114" s="11">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="L114" s="3"/>
       <c r="M114" t="s">
         <v>77</v>
       </c>
       <c r="O114" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -5973,10 +6054,10 @@
         <v>19</v>
       </c>
       <c r="C115" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D115" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="E115" t="s">
         <v>69</v>
@@ -5989,7 +6070,7 @@
         <v>79</v>
       </c>
       <c r="O115" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -6001,10 +6082,10 @@
         <v>19</v>
       </c>
       <c r="C116" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D116" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E116" t="s">
         <v>48</v>
@@ -6017,7 +6098,7 @@
         <v>77</v>
       </c>
       <c r="O116" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -6029,23 +6110,23 @@
         <v>19</v>
       </c>
       <c r="C117" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D117" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E117" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F117" s="11">
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="L117" s="3"/>
       <c r="M117" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O117" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -6057,26 +6138,23 @@
         <v>19</v>
       </c>
       <c r="C118" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D118" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E118" t="s">
         <v>48</v>
       </c>
       <c r="F118" s="11">
-        <v>1</v>
-      </c>
-      <c r="K118" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="L118" s="3"/>
       <c r="M118" t="s">
         <v>77</v>
       </c>
       <c r="O118" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
@@ -6088,30 +6166,89 @@
         <v>19</v>
       </c>
       <c r="C119" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D119" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="E119" t="s">
         <v>48</v>
       </c>
       <c r="F119" s="11">
-        <v>1</v>
-      </c>
-      <c r="K119" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="L119" s="3"/>
       <c r="M119" t="s">
         <v>77</v>
       </c>
       <c r="O119" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C120" t="s">
+        <v>354</v>
+      </c>
+      <c r="D120" t="s">
+        <v>355</v>
+      </c>
+      <c r="E120" t="s">
+        <v>48</v>
+      </c>
+      <c r="F120" s="11">
+        <v>1</v>
+      </c>
+      <c r="K120" t="s">
+        <v>107</v>
+      </c>
+      <c r="L120" s="3"/>
+      <c r="M120" t="s">
+        <v>77</v>
+      </c>
+      <c r="O120" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121" t="s">
+        <v>357</v>
+      </c>
+      <c r="D121" t="s">
+        <v>358</v>
+      </c>
+      <c r="E121" t="s">
+        <v>48</v>
+      </c>
+      <c r="F121" s="11">
+        <v>1</v>
+      </c>
+      <c r="K121" t="s">
+        <v>107</v>
+      </c>
+      <c r="L121" s="3"/>
+      <c r="M121" t="s">
+        <v>77</v>
+      </c>
+      <c r="O121" t="s">
         <v>359</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S119" xr:uid="{129AE431-5806-471D-9C82-A144A32316F7}"/>
+  <autoFilter ref="A1:S121" xr:uid="{129AE431-5806-471D-9C82-A144A32316F7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7994,10 +8131,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A27F77-A36A-4B0F-AB98-73EE4727DE22}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8648,6 +8785,34 @@
       </c>
       <c r="D45" s="16" t="s">
         <v>560</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>583</v>
+      </c>
+      <c r="B46" t="s">
+        <v>576</v>
+      </c>
+      <c r="C46" t="s">
+        <v>580</v>
+      </c>
+      <c r="D46" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>584</v>
+      </c>
+      <c r="B47" t="s">
+        <v>577</v>
+      </c>
+      <c r="C47" t="s">
+        <v>580</v>
+      </c>
+      <c r="D47" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -8692,6 +8857,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="d9de82e3-6650-437c-811c-4330ac3163a7" xsi:nil="true"/>
@@ -8700,15 +8874,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8941,26 +9106,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E58BEAF-C168-4A50-BC01-2C2CE605BA70}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A2FCDB-4CEB-4560-BC24-5417B97B9546}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="d9de82e3-6650-437c-811c-4330ac3163a7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="352660e0-d3e8-47c6-9ec5-fea43b473253"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A2FCDB-4CEB-4560-BC24-5417B97B9546}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E58BEAF-C168-4A50-BC01-2C2CE605BA70}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="d9de82e3-6650-437c-811c-4330ac3163a7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="352660e0-d3e8-47c6-9ec5-fea43b473253"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: having file naming fun; views implemented; deleted exercises; docs: slide verbiage reduced
</commit_message>
<xml_diff>
--- a/metadata/rpharma_specs.xlsx
+++ b/metadata/rpharma_specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phuseaccount.sharepoint.com/sites/Pharmaverse-admiral/Shared Documents/RPharma2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bs832471\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{157F1F95-5780-4369-A8D1-F8AC4BE0C1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03308EDE-FB7F-4602-9BF7-8874DA61D20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="7" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="602">
   <si>
     <t>Attribute</t>
   </si>
@@ -1323,9 +1323,6 @@
   </si>
   <si>
     <t>White</t>
-  </si>
-  <si>
-    <t>Non-White</t>
   </si>
   <si>
     <t>NA</t>
@@ -1910,12 +1907,15 @@
   <si>
     <t>adrg.pdf</t>
   </si>
+  <si>
+    <t>Non-white</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2359,13 +2359,13 @@
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="74.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2428,33 +2428,33 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="62.375" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>392</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>599</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>600</v>
-      </c>
-      <c r="C2" t="s">
-        <v>601</v>
       </c>
     </row>
   </sheetData>
@@ -2472,19 +2472,19 @@
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="58.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="9" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="23.375" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="50.75" customWidth="1"/>
+    <col min="5" max="5" width="58.625" customWidth="1"/>
+    <col min="6" max="6" width="12.375" customWidth="1"/>
+    <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="8" max="9" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2569,33 +2569,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129AE431-5806-471D-9C82-A144A32316F7}">
   <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="9"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.75" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f t="shared" ref="A3:A62" si="0">A2+1</f>
         <v>2</v>
@@ -2718,7 +2718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2752,7 +2752,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2783,7 +2783,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2803,6 +2803,9 @@
       <c r="F6" s="9">
         <v>5</v>
       </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" t="s">
         <v>44</v>
@@ -2811,7 +2814,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2831,6 +2834,9 @@
       <c r="F7" s="9">
         <v>10</v>
       </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
       <c r="K7" t="s">
         <v>68</v>
       </c>
@@ -2839,7 +2845,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2859,6 +2865,9 @@
       <c r="F8" s="9">
         <v>8</v>
       </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
       <c r="K8" t="s">
         <v>73</v>
       </c>
@@ -2867,7 +2876,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2898,7 +2907,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2932,7 +2941,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2952,6 +2961,9 @@
       <c r="F11" s="9">
         <v>3</v>
       </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
       <c r="L11" s="3"/>
       <c r="M11" t="s">
         <v>69</v>
@@ -2960,7 +2972,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2980,6 +2992,9 @@
       <c r="F12" s="9">
         <v>8</v>
       </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
       <c r="K12" s="15" t="s">
         <v>87</v>
       </c>
@@ -2988,7 +3003,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3025,7 +3040,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3062,7 +3077,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3093,7 +3108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3113,6 +3128,9 @@
       <c r="F16" s="9" t="s">
         <v>104</v>
       </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
       <c r="K16" t="s">
         <v>105</v>
       </c>
@@ -3124,7 +3142,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3144,6 +3162,9 @@
       <c r="F17" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
       <c r="K17" t="s">
         <v>109</v>
       </c>
@@ -3152,7 +3173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3186,7 +3207,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3223,7 +3244,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3257,7 +3278,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3294,7 +3315,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f>A21+1</f>
         <v>21</v>
@@ -3331,7 +3352,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3365,7 +3386,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3399,7 +3420,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3433,7 +3454,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3467,7 +3488,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3504,7 +3525,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3538,7 +3559,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3572,7 +3593,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3603,7 +3624,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3637,7 +3658,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3671,7 +3692,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3705,7 +3726,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3736,7 +3757,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3770,7 +3791,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3804,7 +3825,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3835,7 +3856,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3866,7 +3887,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3900,7 +3921,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3934,7 +3955,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3965,7 +3986,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3996,7 +4017,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -4027,7 +4048,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -4058,7 +4079,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -4089,7 +4110,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -4122,7 +4143,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4155,7 +4176,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4185,7 +4206,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4218,7 +4239,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4248,7 +4269,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4278,7 +4299,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -4308,7 +4329,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -4338,7 +4359,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -4369,7 +4390,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -4399,7 +4420,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -4429,7 +4450,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -4459,7 +4480,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -4489,7 +4510,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -4519,7 +4540,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -4553,7 +4574,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -4587,7 +4608,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -4621,7 +4642,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <f t="shared" ref="A63:A118" si="1">A62+1</f>
         <v>62</v>
@@ -4655,7 +4676,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -4689,7 +4710,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -4723,7 +4744,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -4757,7 +4778,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -4791,7 +4812,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -4822,7 +4843,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -4853,7 +4874,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -4884,7 +4905,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -4915,7 +4936,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -4946,7 +4967,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -4977,7 +4998,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -5008,7 +5029,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -5039,7 +5060,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -5070,7 +5091,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -5101,7 +5122,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -5132,7 +5153,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="18" customFormat="1">
+    <row r="79" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -5163,7 +5184,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -5194,7 +5215,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -5225,7 +5246,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -5256,7 +5277,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -5287,7 +5308,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -5318,7 +5339,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -5349,7 +5370,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -5380,7 +5401,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -5411,7 +5432,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -5442,7 +5463,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -5473,7 +5494,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -5504,7 +5525,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -5535,7 +5556,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -5566,7 +5587,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -5594,7 +5615,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -5622,7 +5643,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -5650,7 +5671,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -5675,7 +5696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -5703,7 +5724,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -5731,7 +5752,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -5762,7 +5783,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -5790,7 +5811,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -5818,7 +5839,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -5846,7 +5867,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -5874,7 +5895,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -5902,7 +5923,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -5930,7 +5951,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -5958,7 +5979,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -5986,7 +6007,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -6014,7 +6035,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -6042,7 +6063,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -6070,7 +6091,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -6098,7 +6119,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -6126,7 +6147,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -6154,7 +6175,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -6182,7 +6203,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -6210,7 +6231,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -6238,7 +6259,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -6269,7 +6290,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -6311,30 +6332,30 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="Z28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="3" width="18.75" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="11.75" customWidth="1"/>
+    <col min="7" max="7" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="15.625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
-    <col min="17" max="18" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.75" customWidth="1"/>
+    <col min="11" max="11" width="16.25" customWidth="1"/>
+    <col min="12" max="13" width="12.875" customWidth="1"/>
+    <col min="14" max="14" width="11.75" customWidth="1"/>
+    <col min="15" max="15" width="13.625" customWidth="1"/>
+    <col min="16" max="16" width="15.25" customWidth="1"/>
+    <col min="17" max="18" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -6404,7 +6425,7 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6414,22 +6435,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBC456A-1389-4826-89DD-7A3DE90BCF75}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.25" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="19.625" customWidth="1"/>
     <col min="5" max="5" width="9" style="4"/>
-    <col min="6" max="6" width="59.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.75" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>392</v>
       </c>
@@ -6455,7 +6476,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>87</v>
       </c>
@@ -6477,7 +6498,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>87</v>
       </c>
@@ -6499,7 +6520,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>87</v>
       </c>
@@ -6521,7 +6542,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>87</v>
       </c>
@@ -6543,7 +6564,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -6566,7 +6587,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -6589,7 +6610,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -6612,7 +6633,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -6635,7 +6656,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -6658,7 +6679,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -6681,7 +6702,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -6704,7 +6725,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -6724,7 +6745,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -6744,7 +6765,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -6764,7 +6785,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -6784,7 +6805,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -6804,7 +6825,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -6824,7 +6845,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -6841,7 +6862,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -6855,10 +6876,10 @@
         <v>2</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -6874,11 +6895,8 @@
       <c r="F21" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="H21" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -6895,10 +6913,10 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -6915,10 +6933,10 @@
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -6934,8 +6952,11 @@
       <c r="F24" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="H24" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -6949,10 +6970,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -6966,10 +6987,10 @@
         <v>2</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -6986,7 +7007,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -7003,10 +7024,10 @@
         <v>1</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -7023,10 +7044,10 @@
         <v>2</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -7046,7 +7067,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -7054,7 +7075,7 @@
         <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D31" t="s">
         <v>48</v>
@@ -7063,16 +7084,16 @@
         <v>122</v>
       </c>
       <c r="F31" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="G31" t="s">
         <v>427</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>428</v>
       </c>
-      <c r="H31" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -7080,7 +7101,7 @@
         <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D32" t="s">
         <v>48</v>
@@ -7089,16 +7110,16 @@
         <v>406</v>
       </c>
       <c r="F32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="G32" t="s">
         <v>430</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>431</v>
       </c>
-      <c r="H32" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -7106,7 +7127,7 @@
         <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D33" t="s">
         <v>48</v>
@@ -7115,16 +7136,16 @@
         <v>229</v>
       </c>
       <c r="F33" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="G33" t="s">
         <v>433</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>434</v>
       </c>
-      <c r="H33" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -7132,7 +7153,7 @@
         <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
@@ -7141,21 +7162,21 @@
         <v>421</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="G34" t="s">
         <v>436</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>437</v>
       </c>
-      <c r="H34" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D35" t="s">
         <v>48</v>
@@ -7164,15 +7185,15 @@
         <v>122</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>147</v>
       </c>
       <c r="B36" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D36" t="s">
         <v>48</v>
@@ -7181,15 +7202,15 @@
         <v>406</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D37" t="s">
         <v>48</v>
@@ -7198,32 +7219,32 @@
         <v>3</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D38" t="s">
         <v>48</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D39" t="s">
         <v>72</v>
@@ -7235,15 +7256,15 @@
         <v>122</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D40" t="s">
         <v>72</v>
@@ -7255,58 +7276,58 @@
         <v>406</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D41" t="s">
         <v>72</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F41" s="4">
         <v>3</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D42" t="s">
         <v>72</v>
       </c>
       <c r="E42" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>445</v>
+      </c>
+      <c r="B43" t="s">
         <v>446</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>447</v>
-      </c>
-      <c r="C43" t="s">
-        <v>448</v>
       </c>
       <c r="D43" t="s">
         <v>48</v>
@@ -7315,24 +7336,24 @@
         <v>122</v>
       </c>
       <c r="F43" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="G43" t="s">
         <v>449</v>
-      </c>
-      <c r="G43" t="s">
-        <v>450</v>
       </c>
       <c r="H43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>445</v>
+      </c>
+      <c r="B44" t="s">
         <v>446</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>447</v>
-      </c>
-      <c r="C44" t="s">
-        <v>448</v>
       </c>
       <c r="D44" t="s">
         <v>48</v>
@@ -7341,24 +7362,24 @@
         <v>406</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G44" t="s">
+        <v>450</v>
+      </c>
+      <c r="H44" t="s">
         <v>451</v>
       </c>
-      <c r="H44" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>445</v>
+      </c>
+      <c r="B45" t="s">
         <v>446</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>447</v>
-      </c>
-      <c r="C45" t="s">
-        <v>448</v>
       </c>
       <c r="D45" t="s">
         <v>48</v>
@@ -7367,24 +7388,24 @@
         <v>229</v>
       </c>
       <c r="F45" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="G45" t="s">
         <v>433</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>434</v>
       </c>
-      <c r="H45" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>445</v>
+      </c>
+      <c r="B46" t="s">
         <v>446</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>447</v>
-      </c>
-      <c r="C46" t="s">
-        <v>448</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -7393,24 +7414,24 @@
         <v>421</v>
       </c>
       <c r="F46" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="G46" t="s">
         <v>453</v>
-      </c>
-      <c r="G46" t="s">
-        <v>454</v>
       </c>
       <c r="H46" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>189</v>
       </c>
       <c r="B47" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C47" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D47" t="s">
         <v>48</v>
@@ -7419,18 +7440,18 @@
         <v>122</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D48" t="s">
         <v>48</v>
@@ -7439,21 +7460,21 @@
         <v>122</v>
       </c>
       <c r="F48" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="G48" t="s">
         <v>453</v>
-      </c>
-      <c r="G48" t="s">
-        <v>454</v>
       </c>
       <c r="H48" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D49" t="s">
         <v>48</v>
@@ -7462,24 +7483,24 @@
         <v>406</v>
       </c>
       <c r="F49" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="G49" t="s">
         <v>449</v>
-      </c>
-      <c r="G49" t="s">
-        <v>450</v>
       </c>
       <c r="H49" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B50" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D50" t="s">
         <v>48</v>
@@ -7488,10 +7509,10 @@
         <v>122</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>307</v>
       </c>
@@ -7499,7 +7520,7 @@
         <v>306</v>
       </c>
       <c r="C51" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D51" t="s">
         <v>48</v>
@@ -7508,16 +7529,16 @@
         <v>122</v>
       </c>
       <c r="F51" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="G51" t="s">
         <v>459</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>307</v>
       </c>
@@ -7525,7 +7546,7 @@
         <v>306</v>
       </c>
       <c r="C52" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D52" t="s">
         <v>48</v>
@@ -7534,16 +7555,16 @@
         <v>406</v>
       </c>
       <c r="F52" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="G52" t="s">
         <v>462</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="H52" s="4" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>307</v>
       </c>
@@ -7551,7 +7572,7 @@
         <v>306</v>
       </c>
       <c r="C53" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D53" t="s">
         <v>48</v>
@@ -7560,16 +7581,16 @@
         <v>229</v>
       </c>
       <c r="F53" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G53" t="s">
         <v>465</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>307</v>
       </c>
@@ -7577,7 +7598,7 @@
         <v>306</v>
       </c>
       <c r="C54" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D54" t="s">
         <v>48</v>
@@ -7586,16 +7607,16 @@
         <v>421</v>
       </c>
       <c r="F54" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="G54" t="s">
         <v>468</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="H54" s="4" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>307</v>
       </c>
@@ -7603,7 +7624,7 @@
         <v>306</v>
       </c>
       <c r="C55" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D55" t="s">
         <v>48</v>
@@ -7612,16 +7633,16 @@
         <v>61</v>
       </c>
       <c r="F55" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="G55" t="s">
         <v>471</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="H55" s="4" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>307</v>
       </c>
@@ -7629,7 +7650,7 @@
         <v>306</v>
       </c>
       <c r="C56" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D56" t="s">
         <v>48</v>
@@ -7638,16 +7659,16 @@
         <v>49</v>
       </c>
       <c r="F56" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="G56" t="s">
         <v>474</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="H56" s="4" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>307</v>
       </c>
@@ -7655,25 +7676,25 @@
         <v>306</v>
       </c>
       <c r="C57" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D57" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="G57" t="s">
         <v>478</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="H57" s="4" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>307</v>
       </c>
@@ -7681,7 +7702,7 @@
         <v>306</v>
       </c>
       <c r="C58" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D58" t="s">
         <v>48</v>
@@ -7690,16 +7711,16 @@
         <v>100</v>
       </c>
       <c r="F58" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="G58" t="s">
         <v>481</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="H58" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>307</v>
       </c>
@@ -7707,25 +7728,25 @@
         <v>306</v>
       </c>
       <c r="C59" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D59" t="s">
         <v>48</v>
       </c>
       <c r="E59" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="G59" t="s">
         <v>485</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="H59" s="4" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>313</v>
       </c>
@@ -7733,7 +7754,7 @@
         <v>312</v>
       </c>
       <c r="C60" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D60" t="s">
         <v>48</v>
@@ -7742,13 +7763,13 @@
         <v>122</v>
       </c>
       <c r="F60" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="G60" t="s">
         <v>459</v>
       </c>
-      <c r="G60" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>313</v>
       </c>
@@ -7756,7 +7777,7 @@
         <v>312</v>
       </c>
       <c r="C61" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D61" t="s">
         <v>48</v>
@@ -7765,13 +7786,13 @@
         <v>406</v>
       </c>
       <c r="F61" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="G61" t="s">
         <v>462</v>
       </c>
-      <c r="G61" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>313</v>
       </c>
@@ -7779,7 +7800,7 @@
         <v>312</v>
       </c>
       <c r="C62" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D62" t="s">
         <v>48</v>
@@ -7788,13 +7809,13 @@
         <v>229</v>
       </c>
       <c r="F62" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G62" t="s">
         <v>465</v>
       </c>
-      <c r="G62" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>313</v>
       </c>
@@ -7802,7 +7823,7 @@
         <v>312</v>
       </c>
       <c r="C63" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D63" t="s">
         <v>48</v>
@@ -7811,13 +7832,13 @@
         <v>421</v>
       </c>
       <c r="F63" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="G63" t="s">
         <v>468</v>
       </c>
-      <c r="G63" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>313</v>
       </c>
@@ -7825,7 +7846,7 @@
         <v>312</v>
       </c>
       <c r="C64" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D64" t="s">
         <v>48</v>
@@ -7834,13 +7855,13 @@
         <v>61</v>
       </c>
       <c r="F64" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="G64" t="s">
         <v>471</v>
       </c>
-      <c r="G64" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>313</v>
       </c>
@@ -7848,7 +7869,7 @@
         <v>312</v>
       </c>
       <c r="C65" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D65" t="s">
         <v>48</v>
@@ -7857,13 +7878,13 @@
         <v>49</v>
       </c>
       <c r="F65" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="G65" t="s">
         <v>474</v>
       </c>
-      <c r="G65" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>313</v>
       </c>
@@ -7871,22 +7892,22 @@
         <v>312</v>
       </c>
       <c r="C66" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D66" t="s">
         <v>48</v>
       </c>
       <c r="E66" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="G66" t="s">
         <v>478</v>
       </c>
-      <c r="G66" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>313</v>
       </c>
@@ -7894,7 +7915,7 @@
         <v>312</v>
       </c>
       <c r="C67" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D67" t="s">
         <v>48</v>
@@ -7903,13 +7924,13 @@
         <v>100</v>
       </c>
       <c r="F67" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="G67" t="s">
         <v>481</v>
       </c>
-      <c r="G67" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>313</v>
       </c>
@@ -7917,22 +7938,22 @@
         <v>312</v>
       </c>
       <c r="C68" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D68" t="s">
         <v>48</v>
       </c>
       <c r="E68" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="G68" t="s">
         <v>485</v>
       </c>
-      <c r="G68" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>310</v>
       </c>
@@ -7949,10 +7970,10 @@
         <v>122</v>
       </c>
       <c r="H69" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>310</v>
       </c>
@@ -7969,10 +7990,10 @@
         <v>406</v>
       </c>
       <c r="H70" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>310</v>
       </c>
@@ -7989,10 +8010,10 @@
         <v>229</v>
       </c>
       <c r="H71" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>310</v>
       </c>
@@ -8009,10 +8030,10 @@
         <v>421</v>
       </c>
       <c r="H72" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>310</v>
       </c>
@@ -8029,10 +8050,10 @@
         <v>61</v>
       </c>
       <c r="H73" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>310</v>
       </c>
@@ -8049,10 +8070,10 @@
         <v>49</v>
       </c>
       <c r="H74" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>310</v>
       </c>
@@ -8063,16 +8084,16 @@
         <v>72</v>
       </c>
       <c r="E75" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="H75" t="s">
         <v>477</v>
       </c>
-      <c r="F75" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="H75" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>310</v>
       </c>
@@ -8089,10 +8110,10 @@
         <v>100</v>
       </c>
       <c r="H76" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>310</v>
       </c>
@@ -8103,13 +8124,13 @@
         <v>72</v>
       </c>
       <c r="E77" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="H77" t="s">
         <v>484</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="H77" t="s">
-        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -8123,19 +8144,19 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="25.375" customWidth="1"/>
+    <col min="3" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>392</v>
       </c>
@@ -8146,61 +8167,61 @@
         <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>491</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E2" t="s">
         <v>492</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>491</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>494</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>493</v>
+      </c>
+      <c r="E3" t="s">
         <v>495</v>
       </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>494</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>497</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>496</v>
+      </c>
+      <c r="E4" t="s">
         <v>498</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>497</v>
-      </c>
-      <c r="E4" t="s">
-        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -8213,19 +8234,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A27F77-A36A-4B0F-AB98-73EE4727DE22}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="148.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="46.25" customWidth="1"/>
+    <col min="2" max="2" width="35.625" customWidth="1"/>
+    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="4" max="4" width="148.625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>392</v>
       </c>
@@ -8233,543 +8254,543 @@
         <v>393</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>504</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30.75">
+    <row r="2" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B2" t="s">
         <v>505</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>506</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="11" t="s">
         <v>507</v>
       </c>
-      <c r="D2" s="11" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.5">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>509</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>506</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="C3" t="s">
-        <v>507</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>316</v>
       </c>
       <c r="B4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C4" t="s">
+        <v>506</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="C4" t="s">
-        <v>507</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>316</v>
       </c>
       <c r="B5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>316</v>
       </c>
       <c r="B6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>316</v>
       </c>
       <c r="B7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>316</v>
       </c>
       <c r="B8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>316</v>
       </c>
       <c r="B9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>316</v>
       </c>
       <c r="B10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>316</v>
       </c>
       <c r="B11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>316</v>
       </c>
       <c r="B12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>319</v>
       </c>
       <c r="B13" t="s">
+        <v>521</v>
+      </c>
+      <c r="C13" t="s">
+        <v>506</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="C13" t="s">
-        <v>507</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="42.75">
+    </row>
+    <row r="14" spans="1:8" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>322</v>
       </c>
       <c r="B14" t="s">
+        <v>523</v>
+      </c>
+      <c r="C14" t="s">
+        <v>506</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="C14" t="s">
-        <v>507</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="26.45">
+    </row>
+    <row r="15" spans="1:8" ht="26.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>327</v>
       </c>
       <c r="B15" t="s">
+        <v>525</v>
+      </c>
+      <c r="C15" t="s">
+        <v>506</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="C15" t="s">
-        <v>507</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="58.7" customHeight="1">
+    </row>
+    <row r="16" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>330</v>
       </c>
       <c r="B16" t="s">
+        <v>527</v>
+      </c>
+      <c r="C16" t="s">
+        <v>506</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="C16" t="s">
-        <v>507</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="42.75">
+    </row>
+    <row r="17" spans="1:4" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>333</v>
       </c>
       <c r="B17" t="s">
+        <v>529</v>
+      </c>
+      <c r="C17" t="s">
+        <v>506</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="C17" t="s">
-        <v>507</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="39.4">
+    </row>
+    <row r="18" spans="1:4" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>336</v>
       </c>
       <c r="B18" t="s">
+        <v>531</v>
+      </c>
+      <c r="C18" t="s">
+        <v>506</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="C18" t="s">
-        <v>507</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="91.15">
+    </row>
+    <row r="19" spans="1:4" ht="91.05" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>339</v>
       </c>
       <c r="B19" t="s">
+        <v>533</v>
+      </c>
+      <c r="C19" t="s">
+        <v>506</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="C19" t="s">
-        <v>507</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30.75">
+    </row>
+    <row r="20" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>342</v>
       </c>
       <c r="B20" t="s">
+        <v>535</v>
+      </c>
+      <c r="C20" t="s">
+        <v>506</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="C20" t="s">
-        <v>507</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="57.2">
+    </row>
+    <row r="21" spans="1:4" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>345</v>
       </c>
       <c r="B21" t="s">
+        <v>537</v>
+      </c>
+      <c r="C21" t="s">
+        <v>506</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="C21" t="s">
-        <v>507</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="57.2">
+    </row>
+    <row r="22" spans="1:4" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>348</v>
       </c>
       <c r="B22" t="s">
+        <v>539</v>
+      </c>
+      <c r="C22" t="s">
+        <v>506</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="C22" t="s">
-        <v>507</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="128.44999999999999">
+    </row>
+    <row r="23" spans="1:4" ht="128.4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>351</v>
       </c>
       <c r="B23" t="s">
+        <v>541</v>
+      </c>
+      <c r="C23" t="s">
+        <v>506</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="C23" t="s">
-        <v>507</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.5">
+    </row>
+    <row r="24" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>354</v>
       </c>
       <c r="B24" t="s">
+        <v>543</v>
+      </c>
+      <c r="C24" t="s">
+        <v>506</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C24" t="s">
-        <v>507</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="57.2">
+    </row>
+    <row r="25" spans="1:4" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>357</v>
       </c>
       <c r="B25" t="s">
+        <v>545</v>
+      </c>
+      <c r="C25" t="s">
+        <v>506</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="C25" t="s">
-        <v>507</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="57.2">
+    </row>
+    <row r="26" spans="1:4" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>360</v>
       </c>
       <c r="B26" t="s">
+        <v>547</v>
+      </c>
+      <c r="C26" t="s">
+        <v>506</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="C26" t="s">
-        <v>507</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>363</v>
       </c>
       <c r="B27" t="s">
+        <v>549</v>
+      </c>
+      <c r="C27" t="s">
+        <v>506</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="C27" t="s">
-        <v>507</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="42.75">
+    </row>
+    <row r="28" spans="1:4" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>366</v>
       </c>
       <c r="B28" t="s">
+        <v>551</v>
+      </c>
+      <c r="C28" t="s">
+        <v>506</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="C28" t="s">
-        <v>507</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>369</v>
       </c>
       <c r="B29" t="s">
+        <v>553</v>
+      </c>
+      <c r="C29" t="s">
+        <v>506</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="C29" t="s">
-        <v>507</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>372</v>
       </c>
       <c r="B30" t="s">
+        <v>555</v>
+      </c>
+      <c r="C30" t="s">
+        <v>506</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="C30" t="s">
-        <v>507</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>375</v>
       </c>
       <c r="B31" t="s">
+        <v>557</v>
+      </c>
+      <c r="C31" t="s">
+        <v>506</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C31" t="s">
-        <v>507</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.5">
+    </row>
+    <row r="32" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>378</v>
       </c>
       <c r="B32" t="s">
+        <v>559</v>
+      </c>
+      <c r="C32" t="s">
+        <v>506</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="C32" t="s">
-        <v>507</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>381</v>
       </c>
       <c r="B33" t="s">
+        <v>561</v>
+      </c>
+      <c r="C33" t="s">
+        <v>506</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="C33" t="s">
-        <v>507</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>384</v>
       </c>
       <c r="B34" t="s">
+        <v>563</v>
+      </c>
+      <c r="C34" t="s">
+        <v>506</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="C34" t="s">
-        <v>507</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="91.5">
+    </row>
+    <row r="35" spans="1:4" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>387</v>
       </c>
       <c r="B35" t="s">
+        <v>565</v>
+      </c>
+      <c r="C35" t="s">
+        <v>506</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="C35" t="s">
-        <v>507</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.5">
+    </row>
+    <row r="36" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
       <c r="B36" t="s">
+        <v>567</v>
+      </c>
+      <c r="C36" t="s">
+        <v>506</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="C36" t="s">
-        <v>507</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>225</v>
       </c>
       <c r="B37" t="s">
+        <v>569</v>
+      </c>
+      <c r="C37" t="s">
+        <v>506</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C37" t="s">
-        <v>507</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>183</v>
       </c>
       <c r="B38" t="s">
+        <v>571</v>
+      </c>
+      <c r="C38" t="s">
+        <v>506</v>
+      </c>
+      <c r="D38" s="13" t="s">
         <v>572</v>
       </c>
-      <c r="C38" t="s">
-        <v>507</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>154</v>
       </c>
@@ -8777,13 +8798,13 @@
         <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>148</v>
       </c>
@@ -8791,13 +8812,13 @@
         <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -8805,13 +8826,13 @@
         <v>174</v>
       </c>
       <c r="C41" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>177</v>
       </c>
@@ -8819,13 +8840,13 @@
         <v>177</v>
       </c>
       <c r="C42" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>160</v>
       </c>
@@ -8833,13 +8854,13 @@
         <v>160</v>
       </c>
       <c r="C43" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>168</v>
       </c>
@@ -8847,13 +8868,13 @@
         <v>168</v>
       </c>
       <c r="C44" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -8861,13 +8882,13 @@
         <v>164</v>
       </c>
       <c r="C45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>129</v>
       </c>
@@ -8875,13 +8896,13 @@
         <v>129</v>
       </c>
       <c r="C46" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>171</v>
       </c>
@@ -8889,13 +8910,13 @@
         <v>169</v>
       </c>
       <c r="C47" t="s">
+        <v>581</v>
+      </c>
+      <c r="D47" t="s">
         <v>582</v>
       </c>
-      <c r="D47" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>180</v>
       </c>
@@ -8903,13 +8924,13 @@
         <v>178</v>
       </c>
       <c r="C48" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D48" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -8917,13 +8938,13 @@
         <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D49" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -8931,13 +8952,13 @@
         <v>106</v>
       </c>
       <c r="C50" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D50" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>193</v>
       </c>
@@ -8945,13 +8966,13 @@
         <v>193</v>
       </c>
       <c r="C51" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>196</v>
       </c>
@@ -8959,13 +8980,13 @@
         <v>196</v>
       </c>
       <c r="C52" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>199</v>
       </c>
@@ -8973,13 +8994,13 @@
         <v>199</v>
       </c>
       <c r="C53" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>202</v>
       </c>
@@ -8987,13 +9008,13 @@
         <v>202</v>
       </c>
       <c r="C54" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="57.2">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>205</v>
       </c>
@@ -9001,13 +9022,13 @@
         <v>205</v>
       </c>
       <c r="C55" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>208</v>
       </c>
@@ -9015,13 +9036,13 @@
         <v>208</v>
       </c>
       <c r="C56" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>211</v>
       </c>
@@ -9029,13 +9050,13 @@
         <v>211</v>
       </c>
       <c r="C57" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="28.5">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>214</v>
       </c>
@@ -9043,13 +9064,13 @@
         <v>214</v>
       </c>
       <c r="C58" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>217</v>
       </c>
@@ -9057,13 +9078,13 @@
         <v>217</v>
       </c>
       <c r="C59" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>228</v>
       </c>
@@ -9071,10 +9092,10 @@
         <v>228</v>
       </c>
       <c r="C60" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D60" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -9087,26 +9108,26 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="62.375" customWidth="1"/>
+    <col min="3" max="4" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>392</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>42</v>
@@ -9130,6 +9151,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010018943E1407CCF04989863CF0F432E8B2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db7879c5843627d2d5018033e2f13957">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="352660e0-d3e8-47c6-9ec5-fea43b473253" xmlns:ns3="d9de82e3-6650-437c-811c-4330ac3163a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2446b3d32c0630b69da860c4e69f999" ns2:_="" ns3:_="">
     <xsd:import namespace="352660e0-d3e8-47c6-9ec5-fea43b473253"/>
@@ -9358,23 +9388,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E58BEAF-C168-4A50-BC01-2C2CE605BA70}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E58BEAF-C168-4A50-BC01-2C2CE605BA70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d9de82e3-6650-437c-811c-4330ac3163a7"/>
+    <ds:schemaRef ds:uri="352660e0-d3e8-47c6-9ec5-fea43b473253"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99401450-4116-472E-9386-888FD56A9AF4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A2FCDB-4CEB-4560-BC24-5417B97B9546}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A2FCDB-4CEB-4560-BC24-5417B97B9546}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99401450-4116-472E-9386-888FD56A9AF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="352660e0-d3e8-47c6-9ec5-fea43b473253"/>
+    <ds:schemaRef ds:uri="d9de82e3-6650-437c-811c-4330ac3163a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>